<commit_message>
shoulder & base 2.0
</commit_message>
<xml_diff>
--- a/cad/parameters.xlsx
+++ b/cad/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\workspace\fbd-brachium\cad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EFD003-8B76-4179-B068-0978492D749C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B74B645-6DCC-4074-8E7B-9784D48256AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="3075" windowWidth="15375" windowHeight="7995" xr2:uid="{694E0986-DE7A-453A-AF77-A6ADF57B89A8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6030" windowHeight="10920" xr2:uid="{EBCAEA19-4531-4C06-8052-DD237C6C537F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,15 +30,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
+  <si>
+    <t>base_width</t>
+  </si>
+  <si>
+    <t>base_length</t>
+  </si>
+  <si>
+    <t>turntable_diameter</t>
+  </si>
+  <si>
+    <t>turntable_height</t>
+  </si>
+  <si>
+    <t>turntable_spurs</t>
+  </si>
+  <si>
+    <t>base_height</t>
+  </si>
+  <si>
+    <t>turntable_spur_width</t>
+  </si>
   <si>
     <t>in</t>
   </si>
   <si>
-    <t>turntable_diameter</t>
-  </si>
-  <si>
-    <t>turntable_thickness</t>
+    <t>spine_diameter</t>
+  </si>
+  <si>
+    <t>spine_height</t>
+  </si>
+  <si>
+    <t>ul</t>
   </si>
   <si>
     <t>shoulder_width</t>
@@ -51,75 +74,50 @@
     <t>shoulder_wall_thickness</t>
   </si>
   <si>
-    <t>shoulder_height_offset</t>
-  </si>
-  <si>
-    <t>spine_diameter</t>
-  </si>
-  <si>
-    <t>arm_proximal_gear_diameter</t>
+    <t>shoulder_gear_diameter</t>
   </si>
   <si>
     <t>shoulder_motor_gear_diameter</t>
   </si>
   <si>
-    <t>arm_proximal_gear_thickness</t>
-  </si>
-  <si>
-    <t>arm_proximal_length</t>
-  </si>
-  <si>
-    <t>arm_proximal_width</t>
-  </si>
-  <si>
-    <t>turntable_spur_thickness</t>
-  </si>
-  <si>
-    <t>base_width</t>
-  </si>
-  <si>
-    <t>base_length</t>
-  </si>
-  <si>
-    <t>base_height</t>
-  </si>
-  <si>
-    <t>retention_poles_diameter</t>
+    <t>shoulder_gear_shaft_diameter</t>
+  </si>
+  <si>
+    <t>shoulder_motor_boss</t>
   </si>
   <si>
     <t>turntable_bed_depth</t>
   </si>
   <si>
-    <t>waist_motor_cutout_diameter</t>
-  </si>
-  <si>
-    <t>waist_cutout_overlap</t>
-  </si>
-  <si>
-    <t>base_motor_standoff_thickness</t>
-  </si>
-  <si>
-    <t>base_motor_standoff_length</t>
-  </si>
-  <si>
-    <t>base_motor_standoff_height</t>
-  </si>
-  <si>
-    <t>base_motor_standoff_offset</t>
+    <t>deg</t>
+  </si>
+  <si>
+    <t>base_cutout_diameter</t>
+  </si>
+  <si>
+    <t>base_cutout_contact_angle</t>
+  </si>
+  <si>
+    <t>turntable_motor_support_thickness</t>
+  </si>
+  <si>
+    <t>turntable_motor_support_height</t>
+  </si>
+  <si>
+    <t>turntable_motor_boss</t>
+  </si>
+  <si>
+    <t>turntable_motor_support_width</t>
+  </si>
+  <si>
+    <t>turntable_retention_shaft_diameter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,17 +143,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -466,284 +462,283 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C1014E-165A-444C-A8BF-E9D13287ECB9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60152C37-2222-486C-9F32-1BC2D2297A15}">
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" hidden="1"/>
+    <col min="4" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1">
-        <v>6.5</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
         <v>0.5</v>
       </c>
       <c r="C3" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1">
-        <v>2.5</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1">
-        <v>0.5</v>
+        <v>1.75</v>
       </c>
       <c r="C5" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1">
         <v>0.125</v>
       </c>
       <c r="C6" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1">
-        <v>0</v>
+        <v>1.875</v>
       </c>
       <c r="C7" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1">
-        <v>2</v>
+        <v>0.75</v>
       </c>
       <c r="C8" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="C10" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="B11" s="1">
-        <v>0.25</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B12" s="1">
-        <v>4</v>
+        <v>0.375</v>
       </c>
       <c r="C12" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B13" s="1">
-        <v>0.25</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B14" s="1">
-        <v>0.375</v>
+        <v>0.25</v>
       </c>
       <c r="C14" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1">
-        <v>1.5</v>
+        <v>0.25</v>
       </c>
       <c r="C15" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B16" s="1">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="C16" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B17" s="1">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B18" s="1">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B19" s="1">
-        <v>0.25</v>
+        <v>2.75</v>
       </c>
       <c r="C19" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B20" s="1">
-        <v>2.5</v>
+        <v>0.1875</v>
       </c>
       <c r="C20" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B21" s="1">
-        <v>0.375</v>
+        <v>2.5</v>
       </c>
       <c r="C21" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B22" s="1">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B23" s="1">
-        <v>7</v>
+        <v>0.5</v>
       </c>
       <c r="C23" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B24" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added proximal and distal arms v1, no gear
</commit_message>
<xml_diff>
--- a/cad/parameters.xlsx
+++ b/cad/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\workspace\fbd-brachium\cad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4358DE-4D14-477B-ABCA-3D2D35338615}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646BD60D-FAAD-4809-A5B5-17BC5954ECB2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{EBCAEA19-4531-4C06-8052-DD237C6C537F}"/>
+    <workbookView xWindow="4620" yWindow="1365" windowWidth="15375" windowHeight="7995" xr2:uid="{EBCAEA19-4531-4C06-8052-DD237C6C537F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
   <si>
     <t>base_width</t>
   </si>
@@ -111,6 +111,27 @@
   </si>
   <si>
     <t>turntable_retention_shaft_diameter</t>
+  </si>
+  <si>
+    <t>turntable_retention_shaft_length</t>
+  </si>
+  <si>
+    <t>shoulder_gear_thickness</t>
+  </si>
+  <si>
+    <t>arm_proximal_length</t>
+  </si>
+  <si>
+    <t>arm_distal_length</t>
+  </si>
+  <si>
+    <t>arm_proximal_central_diameter</t>
+  </si>
+  <si>
+    <t>arm_proximal_thickness</t>
+  </si>
+  <si>
+    <t>arm_proximal_motor_boss</t>
   </si>
 </sst>
 </file>
@@ -463,17 +484,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60152C37-2222-486C-9F32-1BC2D2297A15}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
@@ -644,10 +665,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B16" s="1">
-        <v>1.25</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
@@ -655,10 +676,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" s="1">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
@@ -666,10 +687,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B18" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
@@ -677,10 +698,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B19" s="1">
-        <v>2.75</v>
+        <v>2</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
@@ -688,10 +709,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B20" s="1">
-        <v>0.1875</v>
+        <v>2.75</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
@@ -699,10 +720,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21" s="1">
-        <v>2.5</v>
+        <v>0.1875</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
@@ -710,10 +731,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22" s="1">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
@@ -721,10 +742,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B23" s="1">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
@@ -732,12 +753,89 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B24" s="1">
         <v>1</v>
       </c>
       <c r="C24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="1">
+        <v>8</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>